<commit_message>
change some old filenames to GreenVeggie
</commit_message>
<xml_diff>
--- a/Project/Capital-Expenditure.xlsx
+++ b/Project/Capital-Expenditure.xlsx
@@ -5,60 +5,55 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="964" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="2016" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detailed Descriptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mua sensor: cảm biến ánh sáng, nhiệt độ, độ ẩm đất</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mua Arduino Uno Rev3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Làm nhà kính</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vavle dien tu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Module wifi ESP6288</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total:</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Huy</t>
+  </si>
+  <si>
+    <t>Phu</t>
+  </si>
+  <si>
+    <t>Tung</t>
+  </si>
+  <si>
+    <t>Detailed Descriptions</t>
+  </si>
+  <si>
+    <t>Mua sensor: cảm biến ánh sáng, nhiệt độ, độ ẩm đất</t>
+  </si>
+  <si>
+    <t>Mua Arduino Uno Rev3</t>
+  </si>
+  <si>
+    <t>Làm nhà kính</t>
+  </si>
+  <si>
+    <t>Vavle dien tu</t>
+  </si>
+  <si>
+    <t>Module wifi ESP8266</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
 </sst>
 </file>
@@ -66,7 +61,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="166" formatCode="#,##0.000\ [$₫-42A];[RED]\-#,##0.000\ [$₫-42A]"/>
   </numFmts>
@@ -296,7 +291,7 @@
   <dimension ref="B1:H11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -312,6 +307,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0"/>
       <c r="C1" s="0"/>
       <c r="E1" s="0"/>
     </row>
@@ -399,6 +395,7 @@
       <c r="B6" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="C6" s="0"/>
       <c r="D6" s="0" t="s">
         <v>10</v>
       </c>
@@ -409,6 +406,7 @@
       <c r="B7" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="C7" s="0"/>
       <c r="D7" s="0" t="s">
         <v>11</v>
       </c>
@@ -416,8 +414,13 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0"/>
       <c r="E8" s="6"/>
       <c r="H8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0"/>
+      <c r="E9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0"/>

</xml_diff>

<commit_message>
update CapEx for WIFI modules
</commit_message>
<xml_diff>
--- a/Project/Capital-Expenditure.xlsx
+++ b/Project/Capital-Expenditure.xlsx
@@ -5,55 +5,69 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="964" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Huy</t>
-  </si>
-  <si>
-    <t>Phu</t>
-  </si>
-  <si>
-    <t>Tung</t>
-  </si>
-  <si>
-    <t>Detailed Descriptions</t>
-  </si>
-  <si>
-    <t>Mua sensor: cảm biến ánh sáng, nhiệt độ, độ ẩm đất</t>
-  </si>
-  <si>
-    <t>Mua Arduino Uno Rev3</t>
-  </si>
-  <si>
-    <t>Làm nhà kính</t>
-  </si>
-  <si>
-    <t>Vavle dien tu</t>
-  </si>
-  <si>
-    <t>Module wifi ESP8266</t>
-  </si>
-  <si>
-    <t>Total:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detailed Descriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor: cảm biến ánh sáng, nhiệt độ, độ ẩm đất</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35k / 1 sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mua Arduino Uno Rev3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Làm nhà kính</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 mat kinh mica (), 1 mat kinh mica ()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module WIFI ESP8266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMS1117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mach giam ap cho ESP 8266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total:</t>
   </si>
 </sst>
 </file>
@@ -61,7 +75,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="166" formatCode="#,##0.000\ [$₫-42A];[RED]\-#,##0.000\ [$₫-42A]"/>
   </numFmts>
@@ -195,7 +209,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -288,27 +302,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H11"/>
+  <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.38265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.2244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.8061224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="11.8061224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.69897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.1989795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8520408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.4540816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
       <c r="E1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -353,7 +366,9 @@
       <c r="G3" s="6" t="n">
         <v>105</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="n">
@@ -363,7 +378,7 @@
         <v>42478</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="n">
@@ -382,77 +397,91 @@
         <v>42495</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="n">
         <v>260</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="0"/>
+      <c r="C6" s="5" t="n">
+        <v>42515</v>
+      </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="H6" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>90</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>90</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="0"/>
+      <c r="C7" s="5" t="n">
+        <v>42515</v>
+      </c>
       <c r="D7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="H7" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="0"/>
-      <c r="E8" s="6"/>
-      <c r="H8" s="7"/>
+      <c r="E8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="0"/>
-      <c r="E9" s="0"/>
+      <c r="D9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <f aca="true">SUM(INDIRECT(ADDRESS(1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>205</v>
+      </c>
+      <c r="F9" s="9" t="n">
+        <f aca="true">SUM(INDIRECT(ADDRESS(1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>385</v>
+      </c>
+      <c r="G9" s="9" t="n">
+        <f aca="true">SUM(INDIRECT(ADDRESS(1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>635</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="0"/>
-      <c r="D10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="9" t="n">
-        <f aca="true">SUM(INDIRECT(ADDRESS(1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>105</v>
-      </c>
-      <c r="F10" s="9" t="n">
-        <f aca="true">SUM(INDIRECT(ADDRESS(1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>285</v>
-      </c>
-      <c r="G10" s="9" t="n">
-        <f aca="true">SUM(INDIRECT(ADDRESS(1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>545</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="8"/>
-      <c r="E11" s="10" t="n">
-        <f aca="false">SUM(E10:G10)</f>
-        <v>935</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="10" t="n">
+        <f aca="false">SUM(E9:G9)</f>
+        <v>1225</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
update cost for shipping AMS1117
</commit_message>
<xml_diff>
--- a/Project/Capital-Expenditure.xlsx
+++ b/Project/Capital-Expenditure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="1" state="visible" r:id="rId2"/>
@@ -305,23 +305,25 @@
   <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.69897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8520408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.56632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
       <c r="E1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,7 +446,9 @@
       <c r="F7" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="6" t="n">
+        <v>10</v>
+      </c>
       <c r="H7" s="7" t="s">
         <v>14</v>
       </c>
@@ -466,14 +470,14 @@
       </c>
       <c r="G9" s="9" t="n">
         <f aca="true">SUM(INDIRECT(ADDRESS(1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>635</v>
+        <v>645</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="8"/>
       <c r="E10" s="10" t="n">
         <f aca="false">SUM(E9:G9)</f>
-        <v>1225</v>
+        <v>1235</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>

</xml_diff>

<commit_message>
correct cost for shipping AMS1117
</commit_message>
<xml_diff>
--- a/Project/Capital-Expenditure.xlsx
+++ b/Project/Capital-Expenditure.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">AMS1117</t>
   </si>
   <si>
-    <t xml:space="preserve">Mach giam ap cho ESP 8266</t>
+    <t xml:space="preserve">Mach giam ap cho ESP 8266 + Shipping</t>
   </si>
   <si>
     <t xml:space="preserve">Total:</t>
@@ -305,20 +305,20 @@
   <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.56632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.42857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -441,14 +441,12 @@
         <v>13</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G7" s="6" t="n">
-        <v>10</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G7" s="6"/>
       <c r="H7" s="7" t="s">
         <v>14</v>
       </c>
@@ -462,15 +460,15 @@
       </c>
       <c r="E9" s="9" t="n">
         <f aca="true">SUM(INDIRECT(ADDRESS(1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="F9" s="9" t="n">
         <f aca="true">SUM(INDIRECT(ADDRESS(1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="G9" s="9" t="n">
         <f aca="true">SUM(INDIRECT(ADDRESS(1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>645</v>
+        <v>635</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>